<commit_message>
v 0.5 put in message for exceptions, fixed cell wrapping and italics
</commit_message>
<xml_diff>
--- a/F173-A_Template-DyeMINISH Display Data Summary.xlsx
+++ b/F173-A_Template-DyeMINISH Display Data Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kecklund\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpedersen\ReportProject\ReportGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16963B20-74E5-40AC-B7CF-5510C801C30A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2F0254-F164-4F01-A43A-CA6F7C05D173}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26835" windowHeight="8445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,9 +191,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -202,6 +199,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,8 +536,8 @@
   </sheetPr>
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,13 +555,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="180" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -594,16 +594,16 @@
       <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -612,7 +612,7 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -665,7 +665,7 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="5"/>
       <c r="Q6" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>